<commit_message>
Triangle table generation added. Now works only for table_idth == 11
</commit_message>
<xml_diff>
--- a/changed.xlsx
+++ b/changed.xlsx
@@ -6,8 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="template_3x3" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="template_5x5" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="one" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -17,27 +16,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="204"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="36"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="204"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="48"/>
     </font>
   </fonts>
   <fills count="3">
@@ -49,17 +34,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249946592608417"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -69,9 +63,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -83,13 +75,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -367,162 +359,273 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20.7109375" customWidth="1" min="1" max="3"/>
+    <col width="3.7109375" customWidth="1" style="1" min="1" max="23"/>
   </cols>
   <sheetData>
-    <row r="1" ht="99.95" customHeight="1">
-      <c r="A1" s="3" t="n">
+    <row r="1" ht="39.95" customHeight="1">
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="39.95" customHeight="1">
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="O2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="39.95" customHeight="1">
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="P3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="39.95" customHeight="1">
+      <c r="G4" s="2" t="n"/>
+      <c r="H4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="n"/>
+      <c r="N4" s="2" t="n"/>
+      <c r="O4" s="2" t="n"/>
+      <c r="P4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="39.95" customHeight="1">
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="2" t="n"/>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="n"/>
+      <c r="N5" s="2" t="n"/>
+      <c r="O5" s="2" t="n"/>
+      <c r="P5" s="2" t="n"/>
+      <c r="Q5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="39.95" customHeight="1">
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="2" t="n"/>
+      <c r="P6" s="2" t="n"/>
+      <c r="Q6" s="2" t="n"/>
+      <c r="R6" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="S6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="39.95" customHeight="1">
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="2" t="n"/>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="n"/>
+      <c r="N7" s="2" t="n"/>
+      <c r="O7" s="2" t="n"/>
+      <c r="P7" s="2" t="n"/>
+      <c r="Q7" s="2" t="n"/>
+      <c r="R7" s="2" t="n"/>
+      <c r="S7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="T7" s="2" t="n"/>
+    </row>
+    <row r="8" ht="39.95" customHeight="1">
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="2" t="n"/>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M8" s="2" t="n"/>
+      <c r="N8" s="2" t="n"/>
+      <c r="O8" s="2" t="n"/>
+      <c r="P8" s="2" t="n"/>
+      <c r="Q8" s="2" t="n"/>
+      <c r="R8" s="2" t="n"/>
+      <c r="S8" s="2" t="n"/>
+      <c r="T8" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="U8" s="2" t="n"/>
+    </row>
+    <row r="9" ht="39.95" customHeight="1">
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M9" s="2" t="n"/>
+      <c r="N9" s="2" t="n"/>
+      <c r="O9" s="2" t="n"/>
+      <c r="P9" s="2" t="n"/>
+      <c r="Q9" s="2" t="n"/>
+      <c r="R9" s="2" t="n"/>
+      <c r="S9" s="2" t="n"/>
+      <c r="T9" s="2" t="n"/>
+      <c r="U9" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="V9" s="2" t="n"/>
+    </row>
+    <row r="10" ht="39.95" customHeight="1">
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="2" t="n"/>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="M10" s="2" t="n"/>
+      <c r="N10" s="2" t="n"/>
+      <c r="O10" s="2" t="n"/>
+      <c r="P10" s="2" t="n"/>
+      <c r="Q10" s="2" t="n"/>
+      <c r="R10" s="2" t="n"/>
+      <c r="S10" s="2" t="n"/>
+      <c r="T10" s="2" t="n"/>
+      <c r="U10" s="2" t="n"/>
+      <c r="V10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="W10" s="2" t="n"/>
+    </row>
+    <row r="11" ht="39.95" customHeight="1">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" ht="99.95" customHeight="1">
-      <c r="A2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" ht="99.95" customHeight="1">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>7</v>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="W11" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.2362204724409449" right="0.2362204724409449" top="0.7480314960629921" bottom="0.7480314960629921" header="0.3149606299212598" footer="0.3149606299212598"/>
+  <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.7480314960629921" header="0.3149606299212598" footer="0.3149606299212598"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15.7109375" customWidth="1" min="1" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="84.95" customHeight="1">
-      <c r="A1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" ht="84.95" customHeight="1">
-      <c r="A2" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" ht="84.95" customHeight="1">
-      <c r="A3" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" ht="84.95" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="84.95" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.2362204724409449" right="0.2362204724409449" top="0.7480314960629921" bottom="0.7480314960629921" header="0.3149606299212598" footer="0.3149606299212598"/>
-  <pageSetup orientation="portrait" paperSize="9" fitToHeight="0" fitToWidth="0" horizontalDpi="4294967293" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>